<commit_message>
Add soybean height data to tests by making sure data and report variable have the same names
</commit_message>
<xml_diff>
--- a/Tests/Validation/Soybean/Observed.xlsx
+++ b/Tests/Validation/Soybean/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175BE44F-016A-4F54-99C5-047758F0BAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E60BF6-FD45-4B34-82D2-CA4286FE2EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="353">
   <si>
     <t>SimulationName</t>
   </si>
@@ -1103,6 +1103,12 @@
   </si>
   <si>
     <t>Soybean.Leaf.NodeNumber</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.Height</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.Heighterror</t>
   </si>
 </sst>
 </file>
@@ -4048,11 +4054,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR443"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10710" ySplit="570" topLeftCell="H328" activePane="topRight"/>
+    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
+      <pane xSplit="10710" ySplit="570" topLeftCell="H1" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="D324" sqref="D324"/>
+      <selection pane="bottomLeft" activeCell="CF1" sqref="CF1"/>
       <selection pane="bottomRight" activeCell="A337" sqref="A337:AB443"/>
     </sheetView>
   </sheetViews>
@@ -4106,7 +4112,7 @@
     <col min="48" max="48" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="13.86328125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="17" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="8.06640625" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="14" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -4295,7 +4301,7 @@
         <v>161</v>
       </c>
       <c r="AY1" t="s">
-        <v>20</v>
+        <v>351</v>
       </c>
       <c r="AZ1" t="s">
         <v>21</v>
@@ -4394,7 +4400,7 @@
         <v>52</v>
       </c>
       <c r="CF1" t="s">
-        <v>53</v>
+        <v>352</v>
       </c>
       <c r="CG1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Update Observed data using Nconc instead of NConc
</commit_message>
<xml_diff>
--- a/Tests/Validation/Soybean/Observed.xlsx
+++ b/Tests/Validation/Soybean/Observed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Repos\ApsimX\Tests\Validation\Soybean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\Validation\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E60BF6-FD45-4B34-82D2-CA4286FE2EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A46A7D2-3B83-4E59-B020-1EFF7C25808E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28690" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="14" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="354">
   <si>
     <t>SimulationName</t>
   </si>
@@ -730,9 +730,6 @@
     <t>NFixed2</t>
   </si>
   <si>
-    <t>Soybean.Leaf.Nconc</t>
-  </si>
-  <si>
     <t>Soybean.Leaf.N</t>
   </si>
   <si>
@@ -1109,6 +1106,12 @@
   </si>
   <si>
     <t>Soybean.Leaf.Heighterror</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.NConc</t>
+  </si>
+  <si>
+    <t>Soybean.Pod.NConc</t>
   </si>
 </sst>
 </file>
@@ -4054,52 +4057,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CR443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
-      <pane xSplit="10710" ySplit="570" topLeftCell="H1" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="BL1" workbookViewId="0">
+      <pane xSplit="10716" ySplit="576" topLeftCell="H1" activePane="bottomLeft"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="CF1" sqref="CF1"/>
+      <selection pane="bottomLeft" activeCell="BO1" sqref="BO1"/>
       <selection pane="bottomRight" activeCell="A337" sqref="A337:AB443"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="28.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.3984375" customWidth="1"/>
-    <col min="25" max="25" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.44140625" customWidth="1"/>
+    <col min="25" max="25" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" customWidth="1"/>
-    <col min="28" max="29" width="21.86328125" customWidth="1"/>
-    <col min="30" max="30" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="21.88671875" customWidth="1"/>
+    <col min="30" max="30" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="21.6640625" customWidth="1"/>
     <col min="33" max="33" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="18" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="17.6640625" customWidth="1"/>
     <col min="40" max="40" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -4110,43 +4113,43 @@
     <col min="45" max="46" width="20.6640625" customWidth="1"/>
     <col min="47" max="47" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="17" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="6" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="14" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="15" bestFit="1" customWidth="1"/>
     <col min="65" max="65" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="74" max="74" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="79" max="79" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="18" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96">
@@ -4181,7 +4184,7 @@
         <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L1" t="s">
         <v>92</v>
@@ -4193,7 +4196,7 @@
         <v>55</v>
       </c>
       <c r="O1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="P1" t="s">
         <v>91</v>
@@ -4220,7 +4223,7 @@
         <v>157</v>
       </c>
       <c r="X1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Y1" t="s">
         <v>175</v>
@@ -4229,7 +4232,7 @@
         <v>59</v>
       </c>
       <c r="AA1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB1" t="s">
         <v>7</v>
@@ -4244,13 +4247,13 @@
         <v>153</v>
       </c>
       <c r="AF1" t="s">
-        <v>230</v>
+        <v>352</v>
       </c>
       <c r="AG1" t="s">
         <v>152</v>
       </c>
       <c r="AH1" t="s">
-        <v>151</v>
+        <v>353</v>
       </c>
       <c r="AI1" t="s">
         <v>155</v>
@@ -4265,7 +4268,7 @@
         <v>148</v>
       </c>
       <c r="AM1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AN1" t="s">
         <v>150</v>
@@ -4301,7 +4304,7 @@
         <v>161</v>
       </c>
       <c r="AY1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AZ1" t="s">
         <v>21</v>
@@ -4400,7 +4403,7 @@
         <v>52</v>
       </c>
       <c r="CF1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="CG1" t="s">
         <v>54</v>
@@ -4430,13 +4433,13 @@
         <v>207</v>
       </c>
       <c r="CP1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="CQ1" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="CR1" s="26" t="s">
         <v>335</v>
-      </c>
-      <c r="CR1" s="26" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:96">
@@ -12401,7 +12404,7 @@
     </row>
     <row r="237" spans="1:46">
       <c r="A237" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D237" s="4" t="s">
         <v>60</v>
@@ -12415,7 +12418,7 @@
     </row>
     <row r="238" spans="1:46">
       <c r="A238" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D238" s="4" t="s">
         <v>60</v>
@@ -12429,7 +12432,7 @@
     </row>
     <row r="239" spans="1:46">
       <c r="A239" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D239" s="4" t="s">
         <v>60</v>
@@ -12443,7 +12446,7 @@
     </row>
     <row r="240" spans="1:46">
       <c r="A240" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D240" s="4" t="s">
         <v>60</v>
@@ -12457,7 +12460,7 @@
     </row>
     <row r="241" spans="1:8">
       <c r="A241" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D241" s="4" t="s">
         <v>60</v>
@@ -12471,7 +12474,7 @@
     </row>
     <row r="242" spans="1:8">
       <c r="A242" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D242" s="4" t="s">
         <v>60</v>
@@ -12485,7 +12488,7 @@
     </row>
     <row r="243" spans="1:8">
       <c r="A243" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D243" s="4" t="s">
         <v>60</v>
@@ -12499,7 +12502,7 @@
     </row>
     <row r="244" spans="1:8">
       <c r="A244" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D244" s="4" t="s">
         <v>60</v>
@@ -12513,7 +12516,7 @@
     </row>
     <row r="245" spans="1:8">
       <c r="A245" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D245" s="4" t="s">
         <v>60</v>
@@ -12527,7 +12530,7 @@
     </row>
     <row r="246" spans="1:8">
       <c r="A246" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D246" s="4" t="s">
         <v>60</v>
@@ -12541,7 +12544,7 @@
     </row>
     <row r="247" spans="1:8">
       <c r="A247" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D247" s="4" t="s">
         <v>60</v>
@@ -12555,7 +12558,7 @@
     </row>
     <row r="248" spans="1:8">
       <c r="A248" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D248" s="4" t="s">
         <v>60</v>
@@ -12569,7 +12572,7 @@
     </row>
     <row r="249" spans="1:8">
       <c r="A249" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D249" s="4" t="s">
         <v>60</v>
@@ -12583,7 +12586,7 @@
     </row>
     <row r="250" spans="1:8">
       <c r="A250" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D250" s="4" t="s">
         <v>60</v>
@@ -12597,7 +12600,7 @@
     </row>
     <row r="251" spans="1:8">
       <c r="A251" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D251" s="4" t="s">
         <v>60</v>
@@ -12611,7 +12614,7 @@
     </row>
     <row r="252" spans="1:8">
       <c r="A252" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D252" s="4" t="s">
         <v>60</v>
@@ -12625,7 +12628,7 @@
     </row>
     <row r="253" spans="1:8">
       <c r="A253" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D253" s="4" t="s">
         <v>60</v>
@@ -12639,7 +12642,7 @@
     </row>
     <row r="254" spans="1:8">
       <c r="A254" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D254" s="4" t="s">
         <v>60</v>
@@ -12653,7 +12656,7 @@
     </row>
     <row r="255" spans="1:8">
       <c r="A255" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D255" s="4" t="s">
         <v>60</v>
@@ -12667,7 +12670,7 @@
     </row>
     <row r="256" spans="1:8">
       <c r="A256" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D256" s="4" t="s">
         <v>60</v>
@@ -12681,7 +12684,7 @@
     </row>
     <row r="257" spans="1:8">
       <c r="A257" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D257" s="4" t="s">
         <v>60</v>
@@ -12695,7 +12698,7 @@
     </row>
     <row r="258" spans="1:8">
       <c r="A258" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D258" s="4" t="s">
         <v>60</v>
@@ -12709,7 +12712,7 @@
     </row>
     <row r="259" spans="1:8">
       <c r="A259" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D259" s="4" t="s">
         <v>60</v>
@@ -12723,7 +12726,7 @@
     </row>
     <row r="260" spans="1:8">
       <c r="A260" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D260" s="4" t="s">
         <v>60</v>
@@ -12737,7 +12740,7 @@
     </row>
     <row r="261" spans="1:8">
       <c r="A261" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D261" s="4" t="s">
         <v>60</v>
@@ -12751,7 +12754,7 @@
     </row>
     <row r="262" spans="1:8">
       <c r="A262" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D262" s="4" t="s">
         <v>60</v>
@@ -12765,7 +12768,7 @@
     </row>
     <row r="263" spans="1:8">
       <c r="A263" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D263" s="4" t="s">
         <v>60</v>
@@ -12779,7 +12782,7 @@
     </row>
     <row r="264" spans="1:8">
       <c r="A264" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D264" s="4" t="s">
         <v>60</v>
@@ -12793,7 +12796,7 @@
     </row>
     <row r="265" spans="1:8">
       <c r="A265" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D265" s="4" t="s">
         <v>60</v>
@@ -12807,7 +12810,7 @@
     </row>
     <row r="266" spans="1:8">
       <c r="A266" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D266" s="4" t="s">
         <v>60</v>
@@ -12821,7 +12824,7 @@
     </row>
     <row r="267" spans="1:8">
       <c r="A267" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D267" s="4" t="s">
         <v>60</v>
@@ -12835,7 +12838,7 @@
     </row>
     <row r="268" spans="1:8">
       <c r="A268" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D268" s="4" t="s">
         <v>60</v>
@@ -12849,7 +12852,7 @@
     </row>
     <row r="269" spans="1:8">
       <c r="A269" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D269" s="4" t="s">
         <v>60</v>
@@ -12863,7 +12866,7 @@
     </row>
     <row r="270" spans="1:8">
       <c r="A270" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D270" s="4" t="s">
         <v>60</v>
@@ -12877,7 +12880,7 @@
     </row>
     <row r="271" spans="1:8">
       <c r="A271" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D271" s="4" t="s">
         <v>60</v>
@@ -12891,7 +12894,7 @@
     </row>
     <row r="272" spans="1:8">
       <c r="A272" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D272" s="4" t="s">
         <v>60</v>
@@ -12905,7 +12908,7 @@
     </row>
     <row r="273" spans="1:8">
       <c r="A273" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D273" s="4" t="s">
         <v>60</v>
@@ -12919,7 +12922,7 @@
     </row>
     <row r="274" spans="1:8">
       <c r="A274" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D274" s="4" t="s">
         <v>60</v>
@@ -12933,7 +12936,7 @@
     </row>
     <row r="275" spans="1:8">
       <c r="A275" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D275" s="4" t="s">
         <v>60</v>
@@ -12947,7 +12950,7 @@
     </row>
     <row r="276" spans="1:8">
       <c r="A276" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D276" s="4" t="s">
         <v>60</v>
@@ -12961,7 +12964,7 @@
     </row>
     <row r="277" spans="1:8">
       <c r="A277" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D277" s="4" t="s">
         <v>60</v>
@@ -12975,7 +12978,7 @@
     </row>
     <row r="278" spans="1:8">
       <c r="A278" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D278" s="4" t="s">
         <v>60</v>
@@ -12989,7 +12992,7 @@
     </row>
     <row r="279" spans="1:8">
       <c r="A279" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D279" s="4" t="s">
         <v>60</v>
@@ -13003,7 +13006,7 @@
     </row>
     <row r="280" spans="1:8">
       <c r="A280" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D280" s="4" t="s">
         <v>60</v>
@@ -13017,7 +13020,7 @@
     </row>
     <row r="281" spans="1:8">
       <c r="A281" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D281" s="4" t="s">
         <v>60</v>
@@ -13031,7 +13034,7 @@
     </row>
     <row r="282" spans="1:8">
       <c r="A282" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D282" s="4" t="s">
         <v>60</v>
@@ -13045,7 +13048,7 @@
     </row>
     <row r="283" spans="1:8">
       <c r="A283" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D283" s="4" t="s">
         <v>60</v>
@@ -13056,7 +13059,7 @@
     </row>
     <row r="284" spans="1:8">
       <c r="A284" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D284" s="4" t="s">
         <v>60</v>
@@ -13067,7 +13070,7 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D285" s="4" t="s">
         <v>60</v>
@@ -13078,7 +13081,7 @@
     </row>
     <row r="286" spans="1:8">
       <c r="A286" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D286" s="4" t="s">
         <v>60</v>
@@ -13089,7 +13092,7 @@
     </row>
     <row r="287" spans="1:8">
       <c r="A287" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D287" s="4" t="s">
         <v>60</v>
@@ -13103,7 +13106,7 @@
     </row>
     <row r="288" spans="1:8">
       <c r="A288" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D288" s="4" t="s">
         <v>60</v>
@@ -13117,7 +13120,7 @@
     </row>
     <row r="289" spans="1:8">
       <c r="A289" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D289" s="4" t="s">
         <v>60</v>
@@ -13131,7 +13134,7 @@
     </row>
     <row r="290" spans="1:8">
       <c r="A290" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D290" s="4" t="s">
         <v>60</v>
@@ -13145,7 +13148,7 @@
     </row>
     <row r="291" spans="1:8">
       <c r="A291" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D291" s="4" t="s">
         <v>60</v>
@@ -13159,7 +13162,7 @@
     </row>
     <row r="292" spans="1:8">
       <c r="A292" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D292" s="4" t="s">
         <v>60</v>
@@ -13173,7 +13176,7 @@
     </row>
     <row r="293" spans="1:8">
       <c r="A293" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D293" s="4" t="s">
         <v>60</v>
@@ -13187,7 +13190,7 @@
     </row>
     <row r="294" spans="1:8">
       <c r="A294" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D294" s="4" t="s">
         <v>60</v>
@@ -13201,7 +13204,7 @@
     </row>
     <row r="295" spans="1:8">
       <c r="A295" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D295" s="4" t="s">
         <v>60</v>
@@ -13215,7 +13218,7 @@
     </row>
     <row r="296" spans="1:8">
       <c r="A296" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D296" s="4" t="s">
         <v>60</v>
@@ -13226,7 +13229,7 @@
     </row>
     <row r="297" spans="1:8">
       <c r="A297" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D297" s="4" t="s">
         <v>60</v>
@@ -13240,7 +13243,7 @@
     </row>
     <row r="298" spans="1:8">
       <c r="A298" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D298" s="4" t="s">
         <v>60</v>
@@ -13254,7 +13257,7 @@
     </row>
     <row r="299" spans="1:8">
       <c r="A299" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D299" s="4" t="s">
         <v>60</v>
@@ -13268,7 +13271,7 @@
     </row>
     <row r="300" spans="1:8">
       <c r="A300" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D300" s="4" t="s">
         <v>60</v>
@@ -13279,7 +13282,7 @@
     </row>
     <row r="301" spans="1:8">
       <c r="A301" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D301" s="4" t="s">
         <v>60</v>
@@ -13290,7 +13293,7 @@
     </row>
     <row r="302" spans="1:8">
       <c r="A302" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D302" s="4" t="s">
         <v>60</v>
@@ -13301,7 +13304,7 @@
     </row>
     <row r="303" spans="1:8">
       <c r="A303" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D303" s="4" t="s">
         <v>60</v>
@@ -13312,7 +13315,7 @@
     </row>
     <row r="304" spans="1:8">
       <c r="A304" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D304" s="4" t="s">
         <v>60</v>
@@ -13323,7 +13326,7 @@
     </row>
     <row r="305" spans="1:7">
       <c r="A305" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D305" s="4" t="s">
         <v>60</v>
@@ -13334,7 +13337,7 @@
     </row>
     <row r="306" spans="1:7">
       <c r="A306" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D306" s="4" t="s">
         <v>60</v>
@@ -13345,7 +13348,7 @@
     </row>
     <row r="307" spans="1:7">
       <c r="A307" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D307" s="4" t="s">
         <v>60</v>
@@ -13356,7 +13359,7 @@
     </row>
     <row r="308" spans="1:7">
       <c r="A308" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D308" s="4" t="s">
         <v>60</v>
@@ -13367,7 +13370,7 @@
     </row>
     <row r="309" spans="1:7">
       <c r="A309" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D309" s="4" t="s">
         <v>60</v>
@@ -13378,7 +13381,7 @@
     </row>
     <row r="310" spans="1:7">
       <c r="A310" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D310" s="4" t="s">
         <v>60</v>
@@ -13389,7 +13392,7 @@
     </row>
     <row r="311" spans="1:7">
       <c r="A311" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D311" s="4" t="s">
         <v>60</v>
@@ -13400,7 +13403,7 @@
     </row>
     <row r="312" spans="1:7">
       <c r="A312" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D312" s="4" t="s">
         <v>60</v>
@@ -13411,7 +13414,7 @@
     </row>
     <row r="313" spans="1:7">
       <c r="A313" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D313" s="4" t="s">
         <v>60</v>
@@ -13422,7 +13425,7 @@
     </row>
     <row r="314" spans="1:7">
       <c r="A314" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D314" s="4" t="s">
         <v>60</v>
@@ -13433,7 +13436,7 @@
     </row>
     <row r="315" spans="1:7">
       <c r="A315" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D315" s="4" t="s">
         <v>60</v>
@@ -13444,7 +13447,7 @@
     </row>
     <row r="316" spans="1:7">
       <c r="A316" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D316" s="4" t="s">
         <v>60</v>
@@ -13455,7 +13458,7 @@
     </row>
     <row r="317" spans="1:7">
       <c r="A317" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D317" s="4" t="s">
         <v>60</v>
@@ -13466,7 +13469,7 @@
     </row>
     <row r="318" spans="1:7">
       <c r="A318" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D318" s="4" t="s">
         <v>60</v>
@@ -13477,7 +13480,7 @@
     </row>
     <row r="319" spans="1:7">
       <c r="A319" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D319" s="4" t="s">
         <v>60</v>
@@ -13488,7 +13491,7 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D320" s="4" t="s">
         <v>60</v>
@@ -13499,7 +13502,7 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D321" s="4" t="s">
         <v>60</v>
@@ -13510,7 +13513,7 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D322" s="4" t="s">
         <v>60</v>
@@ -13521,7 +13524,7 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D323" s="4" t="s">
         <v>60</v>
@@ -13532,7 +13535,7 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D324" s="4" t="s">
         <v>60</v>
@@ -13543,7 +13546,7 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D325" s="4" t="s">
         <v>60</v>
@@ -13554,7 +13557,7 @@
     </row>
     <row r="326" spans="1:7">
       <c r="A326" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D326" s="4" t="s">
         <v>60</v>
@@ -13565,7 +13568,7 @@
     </row>
     <row r="327" spans="1:7">
       <c r="A327" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D327" s="4" t="s">
         <v>60</v>
@@ -13576,7 +13579,7 @@
     </row>
     <row r="328" spans="1:7">
       <c r="A328" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D328" s="4" t="s">
         <v>60</v>
@@ -13587,7 +13590,7 @@
     </row>
     <row r="329" spans="1:7">
       <c r="A329" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D329" s="4" t="s">
         <v>60</v>
@@ -13598,7 +13601,7 @@
     </row>
     <row r="330" spans="1:7">
       <c r="A330" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D330" s="4" t="s">
         <v>60</v>
@@ -13609,7 +13612,7 @@
     </row>
     <row r="331" spans="1:7">
       <c r="A331" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D331" s="4" t="s">
         <v>60</v>
@@ -13620,7 +13623,7 @@
     </row>
     <row r="332" spans="1:7">
       <c r="A332" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D332" s="4" t="s">
         <v>60</v>
@@ -13631,7 +13634,7 @@
     </row>
     <row r="333" spans="1:7">
       <c r="A333" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D333" s="4" t="s">
         <v>60</v>
@@ -13642,7 +13645,7 @@
     </row>
     <row r="334" spans="1:7">
       <c r="A334" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D334" s="4" t="s">
         <v>60</v>
@@ -13653,7 +13656,7 @@
     </row>
     <row r="335" spans="1:7">
       <c r="A335" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D335" s="4" t="s">
         <v>60</v>
@@ -13664,7 +13667,7 @@
     </row>
     <row r="336" spans="1:7">
       <c r="A336" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D336" s="4" t="s">
         <v>60</v>
@@ -13675,7 +13678,7 @@
     </row>
     <row r="337" spans="1:44">
       <c r="A337" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B337" s="29">
         <v>41847</v>
@@ -13720,7 +13723,7 @@
     </row>
     <row r="338" spans="1:44">
       <c r="A338" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B338" s="29">
         <v>41860</v>
@@ -13765,7 +13768,7 @@
     </row>
     <row r="339" spans="1:44">
       <c r="A339" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B339" s="29">
         <v>41863</v>
@@ -13803,7 +13806,7 @@
     </row>
     <row r="340" spans="1:44">
       <c r="A340" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B340" s="29">
         <v>41875</v>
@@ -13847,7 +13850,7 @@
     </row>
     <row r="341" spans="1:44">
       <c r="A341" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B341" s="29">
         <v>41888</v>
@@ -13893,7 +13896,7 @@
     </row>
     <row r="342" spans="1:44">
       <c r="A342" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B342" s="29">
         <v>41890</v>
@@ -13929,7 +13932,7 @@
     </row>
     <row r="343" spans="1:44">
       <c r="A343" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B343" s="29">
         <v>41904</v>
@@ -13975,7 +13978,7 @@
     </row>
     <row r="344" spans="1:44">
       <c r="A344" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B344" s="29">
         <v>41919</v>
@@ -14021,7 +14024,7 @@
     </row>
     <row r="345" spans="1:44">
       <c r="A345" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B345" s="29">
         <v>41934</v>
@@ -14067,7 +14070,7 @@
     </row>
     <row r="346" spans="1:44">
       <c r="A346" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B346" s="29">
         <v>42218</v>
@@ -14111,7 +14114,7 @@
     </row>
     <row r="347" spans="1:44">
       <c r="A347" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B347" s="29">
         <v>42228</v>
@@ -14149,7 +14152,7 @@
     </row>
     <row r="348" spans="1:44">
       <c r="A348" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B348" s="29">
         <v>42232</v>
@@ -14193,7 +14196,7 @@
     </row>
     <row r="349" spans="1:44">
       <c r="A349" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B349" s="29">
         <v>42246</v>
@@ -14237,7 +14240,7 @@
     </row>
     <row r="350" spans="1:44">
       <c r="A350" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B350" s="29">
         <v>42255</v>
@@ -14273,7 +14276,7 @@
     </row>
     <row r="351" spans="1:44">
       <c r="A351" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B351" s="29">
         <v>42260</v>
@@ -14319,7 +14322,7 @@
     </row>
     <row r="352" spans="1:44">
       <c r="A352" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B352" s="29">
         <v>42274</v>
@@ -14365,7 +14368,7 @@
     </row>
     <row r="353" spans="1:28">
       <c r="A353" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B353" s="29">
         <v>42288</v>
@@ -14411,7 +14414,7 @@
     </row>
     <row r="354" spans="1:28">
       <c r="A354" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B354" s="29">
         <v>42299</v>
@@ -14457,7 +14460,7 @@
     </row>
     <row r="355" spans="1:28">
       <c r="A355" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B355" s="29">
         <v>42571</v>
@@ -14501,7 +14504,7 @@
     </row>
     <row r="356" spans="1:28">
       <c r="A356" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B356" s="29">
         <v>42584</v>
@@ -14545,7 +14548,7 @@
     </row>
     <row r="357" spans="1:28">
       <c r="A357" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B357" s="29">
         <v>42591</v>
@@ -14589,7 +14592,7 @@
     </row>
     <row r="358" spans="1:28">
       <c r="A358" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B358" s="29">
         <v>42594</v>
@@ -14627,7 +14630,7 @@
     </row>
     <row r="359" spans="1:28">
       <c r="A359" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B359" s="29">
         <v>42598</v>
@@ -14671,7 +14674,7 @@
     </row>
     <row r="360" spans="1:28">
       <c r="A360" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B360" s="29">
         <v>42605</v>
@@ -14715,7 +14718,7 @@
     </row>
     <row r="361" spans="1:28">
       <c r="A361" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B361" s="29">
         <v>42612</v>
@@ -14761,7 +14764,7 @@
     </row>
     <row r="362" spans="1:28">
       <c r="A362" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B362" s="29">
         <v>42621</v>
@@ -14797,7 +14800,7 @@
     </row>
     <row r="363" spans="1:28">
       <c r="A363" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B363" s="29">
         <v>42628</v>
@@ -14843,7 +14846,7 @@
     </row>
     <row r="364" spans="1:28">
       <c r="A364" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B364" s="29">
         <v>42643</v>
@@ -14889,7 +14892,7 @@
     </row>
     <row r="365" spans="1:28">
       <c r="A365" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B365" s="29">
         <v>42665</v>
@@ -14935,7 +14938,7 @@
     </row>
     <row r="366" spans="1:28">
       <c r="A366" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B366" s="29">
         <v>41847</v>
@@ -14979,7 +14982,7 @@
     </row>
     <row r="367" spans="1:28">
       <c r="A367" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B367" s="29">
         <v>41860</v>
@@ -15023,7 +15026,7 @@
     </row>
     <row r="368" spans="1:28">
       <c r="A368" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B368" s="29">
         <v>41867</v>
@@ -15061,7 +15064,7 @@
     </row>
     <row r="369" spans="1:28">
       <c r="A369" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B369" s="29">
         <v>41875</v>
@@ -15105,7 +15108,7 @@
     </row>
     <row r="370" spans="1:28">
       <c r="A370" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B370" s="29">
         <v>41888</v>
@@ -15151,7 +15154,7 @@
     </row>
     <row r="371" spans="1:28">
       <c r="A371" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B371" s="29">
         <v>41894</v>
@@ -15187,7 +15190,7 @@
     </row>
     <row r="372" spans="1:28">
       <c r="A372" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B372" s="29">
         <v>41904</v>
@@ -15233,7 +15236,7 @@
     </row>
     <row r="373" spans="1:28">
       <c r="A373" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B373" s="29">
         <v>41919</v>
@@ -15279,7 +15282,7 @@
     </row>
     <row r="374" spans="1:28">
       <c r="A374" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B374" s="29">
         <v>41934</v>
@@ -15315,7 +15318,7 @@
     </row>
     <row r="375" spans="1:28">
       <c r="A375" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B375" s="29">
         <v>41944</v>
@@ -15361,7 +15364,7 @@
     </row>
     <row r="376" spans="1:28">
       <c r="A376" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B376" s="29">
         <v>42218</v>
@@ -15405,7 +15408,7 @@
     </row>
     <row r="377" spans="1:28">
       <c r="A377" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B377" s="29">
         <v>42232</v>
@@ -15451,7 +15454,7 @@
     </row>
     <row r="378" spans="1:28">
       <c r="A378" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B378" s="29">
         <v>42246</v>
@@ -15495,7 +15498,7 @@
     </row>
     <row r="379" spans="1:28">
       <c r="A379" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B379" s="29">
         <v>42260</v>
@@ -15541,7 +15544,7 @@
     </row>
     <row r="380" spans="1:28">
       <c r="A380" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B380" s="29">
         <v>42274</v>
@@ -15587,7 +15590,7 @@
     </row>
     <row r="381" spans="1:28">
       <c r="A381" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B381" s="29">
         <v>42288</v>
@@ -15633,7 +15636,7 @@
     </row>
     <row r="382" spans="1:28">
       <c r="A382" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B382" s="29">
         <v>42299</v>
@@ -15669,7 +15672,7 @@
     </row>
     <row r="383" spans="1:28">
       <c r="A383" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B383" s="29">
         <v>42309</v>
@@ -15715,7 +15718,7 @@
     </row>
     <row r="384" spans="1:28">
       <c r="A384" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B384" s="29">
         <v>42571</v>
@@ -15759,7 +15762,7 @@
     </row>
     <row r="385" spans="1:28">
       <c r="A385" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B385" s="29">
         <v>42584</v>
@@ -15803,7 +15806,7 @@
     </row>
     <row r="386" spans="1:28">
       <c r="A386" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B386" s="29">
         <v>42591</v>
@@ -15847,7 +15850,7 @@
     </row>
     <row r="387" spans="1:28">
       <c r="A387" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B387" s="29">
         <v>42598</v>
@@ -15893,7 +15896,7 @@
     </row>
     <row r="388" spans="1:28">
       <c r="A388" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B388" s="29">
         <v>42605</v>
@@ -15937,7 +15940,7 @@
     </row>
     <row r="389" spans="1:28">
       <c r="A389" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B389" s="29">
         <v>42612</v>
@@ -15983,7 +15986,7 @@
     </row>
     <row r="390" spans="1:28">
       <c r="A390" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B390" s="29">
         <v>42625</v>
@@ -16019,7 +16022,7 @@
     </row>
     <row r="391" spans="1:28">
       <c r="A391" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B391" s="29">
         <v>42628</v>
@@ -16065,7 +16068,7 @@
     </row>
     <row r="392" spans="1:28">
       <c r="A392" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B392" s="29">
         <v>42643</v>
@@ -16111,7 +16114,7 @@
     </row>
     <row r="393" spans="1:28">
       <c r="A393" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B393" s="29">
         <v>42665</v>
@@ -16147,7 +16150,7 @@
     </row>
     <row r="394" spans="1:28">
       <c r="A394" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B394" s="29">
         <v>42675</v>
@@ -16193,7 +16196,7 @@
     </row>
     <row r="395" spans="1:28">
       <c r="A395" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B395" s="29">
         <v>41847</v>
@@ -16237,7 +16240,7 @@
     </row>
     <row r="396" spans="1:28">
       <c r="A396" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B396" s="29">
         <v>41860</v>
@@ -16283,7 +16286,7 @@
     </row>
     <row r="397" spans="1:28">
       <c r="A397" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B397" s="29">
         <v>41875</v>
@@ -16327,7 +16330,7 @@
     </row>
     <row r="398" spans="1:28">
       <c r="A398" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B398" s="29">
         <v>41885</v>
@@ -16363,7 +16366,7 @@
     </row>
     <row r="399" spans="1:28">
       <c r="A399" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B399" s="29">
         <v>41888</v>
@@ -16409,7 +16412,7 @@
     </row>
     <row r="400" spans="1:28">
       <c r="A400" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B400" s="29">
         <v>41904</v>
@@ -16455,7 +16458,7 @@
     </row>
     <row r="401" spans="1:28">
       <c r="A401" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B401" s="29">
         <v>41919</v>
@@ -16501,7 +16504,7 @@
     </row>
     <row r="402" spans="1:28">
       <c r="A402" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B402" s="29">
         <v>42218</v>
@@ -16545,7 +16548,7 @@
     </row>
     <row r="403" spans="1:28">
       <c r="A403" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B403" s="29">
         <v>42225</v>
@@ -16583,7 +16586,7 @@
     </row>
     <row r="404" spans="1:28">
       <c r="A404" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B404" s="29">
         <v>42232</v>
@@ -16627,7 +16630,7 @@
     </row>
     <row r="405" spans="1:28">
       <c r="A405" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B405" s="29">
         <v>42246</v>
@@ -16673,7 +16676,7 @@
     </row>
     <row r="406" spans="1:28">
       <c r="A406" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B406" s="29">
         <v>42260</v>
@@ -16719,7 +16722,7 @@
     </row>
     <row r="407" spans="1:28">
       <c r="A407" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B407" s="29">
         <v>42274</v>
@@ -16765,7 +16768,7 @@
     </row>
     <row r="408" spans="1:28">
       <c r="A408" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B408" s="29">
         <v>42284</v>
@@ -16801,7 +16804,7 @@
     </row>
     <row r="409" spans="1:28">
       <c r="A409" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B409" s="29">
         <v>42288</v>
@@ -16847,7 +16850,7 @@
     </row>
     <row r="410" spans="1:28">
       <c r="A410" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B410" s="29">
         <v>42571</v>
@@ -16891,7 +16894,7 @@
     </row>
     <row r="411" spans="1:28">
       <c r="A411" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B411" s="29">
         <v>42584</v>
@@ -16935,7 +16938,7 @@
     </row>
     <row r="412" spans="1:28">
       <c r="A412" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B412" s="29">
         <v>42591</v>
@@ -16981,7 +16984,7 @@
     </row>
     <row r="413" spans="1:28">
       <c r="A413" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B413" s="29">
         <v>42598</v>
@@ -17025,7 +17028,7 @@
     </row>
     <row r="414" spans="1:28">
       <c r="A414" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B414" s="29">
         <v>42605</v>
@@ -17071,7 +17074,7 @@
     </row>
     <row r="415" spans="1:28">
       <c r="A415" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B415" s="29">
         <v>42612</v>
@@ -17117,7 +17120,7 @@
     </row>
     <row r="416" spans="1:28">
       <c r="A416" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B416" s="29">
         <v>42616</v>
@@ -17153,7 +17156,7 @@
     </row>
     <row r="417" spans="1:28">
       <c r="A417" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B417" s="29">
         <v>42628</v>
@@ -17199,7 +17202,7 @@
     </row>
     <row r="418" spans="1:28">
       <c r="A418" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B418" s="29">
         <v>42643</v>
@@ -17255,7 +17258,7 @@
     </row>
     <row r="419" spans="1:28">
       <c r="A419" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B419" s="33">
         <v>41463</v>
@@ -17293,7 +17296,7 @@
     </row>
     <row r="420" spans="1:28">
       <c r="A420" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B420" s="33">
         <v>41476</v>
@@ -17331,7 +17334,7 @@
     </row>
     <row r="421" spans="1:28">
       <c r="A421" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B421" s="33">
         <v>41478</v>
@@ -17367,7 +17370,7 @@
     </row>
     <row r="422" spans="1:28">
       <c r="A422" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B422" s="33">
         <v>41481</v>
@@ -17405,7 +17408,7 @@
     </row>
     <row r="423" spans="1:28">
       <c r="A423" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B423" s="33">
         <v>41488</v>
@@ -17443,7 +17446,7 @@
     </row>
     <row r="424" spans="1:28">
       <c r="A424" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B424" s="33">
         <v>41493</v>
@@ -17479,7 +17482,7 @@
     </row>
     <row r="425" spans="1:28">
       <c r="A425" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B425" s="33">
         <v>41502</v>
@@ -17517,7 +17520,7 @@
     </row>
     <row r="426" spans="1:28">
       <c r="A426" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B426" s="33">
         <v>41505</v>
@@ -17553,7 +17556,7 @@
     </row>
     <row r="427" spans="1:28">
       <c r="A427" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B427" s="33">
         <v>41517</v>
@@ -17591,7 +17594,7 @@
     </row>
     <row r="428" spans="1:28">
       <c r="A428" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B428" s="33">
         <v>41522</v>
@@ -17627,7 +17630,7 @@
     </row>
     <row r="429" spans="1:28">
       <c r="A429" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B429" s="33">
         <v>41533</v>
@@ -17665,7 +17668,7 @@
     </row>
     <row r="430" spans="1:28">
       <c r="A430" s="27" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B430" s="33">
         <v>41543</v>
@@ -17713,7 +17716,7 @@
     </row>
     <row r="431" spans="1:28">
       <c r="A431" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B431" s="33">
         <v>41826</v>
@@ -17751,7 +17754,7 @@
     </row>
     <row r="432" spans="1:28">
       <c r="A432" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B432" s="33">
         <v>41839</v>
@@ -17789,7 +17792,7 @@
     </row>
     <row r="433" spans="1:28">
       <c r="A433" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B433" s="33">
         <v>41846</v>
@@ -17827,7 +17830,7 @@
     </row>
     <row r="434" spans="1:28">
       <c r="A434" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B434" s="33">
         <v>41853</v>
@@ -17865,7 +17868,7 @@
     </row>
     <row r="435" spans="1:28">
       <c r="A435" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B435" s="33">
         <v>41865</v>
@@ -17903,7 +17906,7 @@
     </row>
     <row r="436" spans="1:28">
       <c r="A436" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B436" s="33">
         <v>41879</v>
@@ -17941,7 +17944,7 @@
     </row>
     <row r="437" spans="1:28">
       <c r="A437" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B437" s="33">
         <v>41899</v>
@@ -17979,7 +17982,7 @@
     </row>
     <row r="438" spans="1:28">
       <c r="A438" s="27" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B438" s="33">
         <v>41910</v>
@@ -18027,7 +18030,7 @@
     </row>
     <row r="439" spans="1:28">
       <c r="A439" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B439" s="33">
         <v>42208</v>
@@ -18067,7 +18070,7 @@
     </row>
     <row r="440" spans="1:28">
       <c r="A440" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B440" s="33">
         <v>42226</v>
@@ -18107,7 +18110,7 @@
     </row>
     <row r="441" spans="1:28">
       <c r="A441" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B441" s="33">
         <v>42241</v>
@@ -18145,7 +18148,7 @@
     </row>
     <row r="442" spans="1:28">
       <c r="A442" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B442" s="33">
         <v>42257</v>
@@ -18183,7 +18186,7 @@
     </row>
     <row r="443" spans="1:28">
       <c r="A443" s="27" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B443" s="33">
         <v>42273</v>
@@ -18242,9 +18245,9 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45">
@@ -19703,12 +19706,12 @@
       <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="13" max="13" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.06640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.06640625" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:24">
@@ -22446,19 +22449,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53125" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23131,41 +23134,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="28.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.6640625" customWidth="1"/>
-    <col min="14" max="14" width="14.06640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="21.86328125" customWidth="1"/>
-    <col min="28" max="28" width="20.53125" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="21.88671875" customWidth="1"/>
+    <col min="28" max="28" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="18" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -23174,43 +23177,43 @@
     <col min="40" max="40" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="17" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.06640625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="14" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.53125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="6.53125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="15" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="67" max="67" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="68" max="68" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.06640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="76" max="76" width="18" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:87">

</xml_diff>